<commit_message>
data till 7 july 9AM
</commit_message>
<xml_diff>
--- a/JioMobile/July2021Mobile.xlsx
+++ b/JioMobile/July2021Mobile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7965" activeTab="2"/>
+    <workbookView windowWidth="19815" windowHeight="7815" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Orders" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="268">
   <si>
     <t>S.No.</t>
   </si>
@@ -429,6 +429,9 @@
     <t>amrit phone ghar (660850063)</t>
   </si>
   <si>
+    <t>GANGA COMMUNICATION (661712658)</t>
+  </si>
+  <si>
     <t>GUDDU MOBILE SHOP (661670780)</t>
   </si>
   <si>
@@ -813,7 +816,13 @@
     <t>Dues Amount</t>
   </si>
   <si>
+    <t>Kaler Zone Retailers ( Jio Phone dues) =&gt;&gt;</t>
+  </si>
+  <si>
     <t>Tabakala</t>
+  </si>
+  <si>
+    <t>ARWAL ZONE RETAILERS ( Jio phone dues) =&gt;&gt;</t>
   </si>
 </sst>
 </file>
@@ -822,10 +831,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="[$-409]d\-mmm;@"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -851,6 +860,57 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -867,39 +927,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -915,7 +945,44 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -930,68 +997,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1070,7 +1079,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1082,19 +1097,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1106,19 +1109,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1136,19 +1145,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1166,6 +1169,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1178,13 +1187,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1196,19 +1217,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1220,7 +1229,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1232,13 +1247,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1267,50 +1276,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1326,17 +1291,29 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1358,9 +1335,41 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1369,7 +1378,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1387,130 +1396,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="23" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1965,11 +1974,11 @@
   <dimension ref="A1:AX175"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="8" ySplit="2" topLeftCell="I149" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="2" topLeftCell="K93" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L154" sqref="L154"/>
+      <selection pane="bottomRight" activeCell="O103" sqref="O103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -2119,26 +2128,26 @@
       <c r="A2" s="20"/>
       <c r="B2" s="30">
         <f>SUM(F3:F1000)</f>
-        <v>110500</v>
+        <v>131500</v>
       </c>
       <c r="D2" s="21">
         <f>SUM(H3:H1000)</f>
-        <v>30000</v>
+        <v>51000</v>
       </c>
       <c r="E2" s="22" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="31">
         <f>H2+I2</f>
-        <v>110500</v>
+        <v>131500</v>
       </c>
       <c r="G2" s="31">
         <f>H2/1500</f>
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="H2" s="21">
         <f>SUM(J2:AN2)</f>
-        <v>30000</v>
+        <v>51000</v>
       </c>
       <c r="I2" s="25">
         <f>SUM(I3:I1000)</f>
@@ -2162,11 +2171,11 @@
       </c>
       <c r="N2" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="O2" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="P2" s="25">
         <f t="shared" si="0"/>
@@ -3791,15 +3800,15 @@
       </c>
       <c r="F25" s="18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="G25" s="18">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" s="18">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="I25" s="35">
         <v>0</v>
@@ -3808,7 +3817,10 @@
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
+      <c r="N25" s="1">
+        <f>1*1500</f>
+        <v>1500</v>
+      </c>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
@@ -5137,15 +5149,15 @@
       </c>
       <c r="F45" s="18">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="G45" s="18">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H45" s="18">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="I45" s="35">
         <v>0</v>
@@ -5154,7 +5166,10 @@
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
-      <c r="N45" s="1"/>
+      <c r="N45" s="1">
+        <f>2*1500</f>
+        <v>3000</v>
+      </c>
       <c r="O45" s="1"/>
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
@@ -5408,15 +5423,15 @@
       </c>
       <c r="F49" s="18">
         <f t="shared" si="4"/>
-        <v>4500</v>
+        <v>7500</v>
       </c>
       <c r="G49" s="18">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H49" s="18">
         <f t="shared" si="6"/>
-        <v>4500</v>
+        <v>7500</v>
       </c>
       <c r="I49" s="35">
         <v>0</v>
@@ -5428,7 +5443,10 @@
         <v>4500</v>
       </c>
       <c r="M49" s="1"/>
-      <c r="N49" s="1"/>
+      <c r="N49" s="1">
+        <f>2*1500</f>
+        <v>3000</v>
+      </c>
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
       <c r="Q49" s="1"/>
@@ -8897,17 +8915,20 @@
       <c r="D101" s="12" t="s">
         <v>133</v>
       </c>
+      <c r="E101" s="12" t="s">
+        <v>136</v>
+      </c>
       <c r="F101" s="18">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="G101" s="18">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H101" s="18">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="I101" s="35">
         <v>0</v>
@@ -8917,7 +8938,10 @@
       <c r="L101" s="1"/>
       <c r="M101" s="1"/>
       <c r="N101" s="1"/>
-      <c r="O101" s="1"/>
+      <c r="O101" s="1">
+        <f>2*1500</f>
+        <v>3000</v>
+      </c>
       <c r="P101" s="1"/>
       <c r="Q101" s="1"/>
       <c r="R101" s="1"/>
@@ -8962,7 +8986,7 @@
         <v>133</v>
       </c>
       <c r="E102" s="12" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F102" s="18">
         <f t="shared" si="10"/>
@@ -9026,25 +9050,25 @@
         <v>100</v>
       </c>
       <c r="B103" s="12" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D103" s="12" t="s">
         <v>133</v>
       </c>
       <c r="E103" s="12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F103" s="18">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="G103" s="18">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H103" s="18">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="I103" s="35">
         <v>0</v>
@@ -9054,7 +9078,10 @@
       <c r="L103" s="1"/>
       <c r="M103" s="1"/>
       <c r="N103" s="1"/>
-      <c r="O103" s="1"/>
+      <c r="O103" s="1">
+        <f>2*1500</f>
+        <v>3000</v>
+      </c>
       <c r="P103" s="1"/>
       <c r="Q103" s="1"/>
       <c r="R103" s="1"/>
@@ -9096,13 +9123,13 @@
         <v>101</v>
       </c>
       <c r="B104" s="12" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="D104" s="12" t="s">
         <v>133</v>
       </c>
       <c r="E104" s="12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F104" s="18">
         <f t="shared" si="10"/>
@@ -9233,7 +9260,7 @@
         <v>133</v>
       </c>
       <c r="E106" s="12" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F106" s="18">
         <f t="shared" si="10"/>
@@ -9297,25 +9324,25 @@
         <v>104</v>
       </c>
       <c r="B107" s="12" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D107" s="12" t="s">
         <v>133</v>
       </c>
       <c r="E107" s="12" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F107" s="18">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="G107" s="18">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H107" s="18">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="I107" s="35">
         <v>0</v>
@@ -9324,7 +9351,10 @@
       <c r="K107" s="1"/>
       <c r="L107" s="1"/>
       <c r="M107" s="1"/>
-      <c r="N107" s="1"/>
+      <c r="N107" s="1">
+        <f>2*1500</f>
+        <v>3000</v>
+      </c>
       <c r="O107" s="1"/>
       <c r="P107" s="1"/>
       <c r="Q107" s="1"/>
@@ -9370,7 +9400,7 @@
         <v>133</v>
       </c>
       <c r="E108" s="12" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F108" s="18">
         <f t="shared" si="10"/>
@@ -9437,7 +9467,7 @@
         <v>133</v>
       </c>
       <c r="E109" s="12" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F109" s="18">
         <f t="shared" si="10"/>
@@ -9504,7 +9534,7 @@
         <v>133</v>
       </c>
       <c r="E110" s="12" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F110" s="18">
         <f t="shared" si="10"/>
@@ -9568,13 +9598,13 @@
         <v>108</v>
       </c>
       <c r="B111" s="12" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D111" s="12" t="s">
         <v>133</v>
       </c>
       <c r="E111" s="12" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F111" s="18">
         <f t="shared" si="10"/>
@@ -9637,13 +9667,13 @@
         <v>109</v>
       </c>
       <c r="B112" s="12" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D112" s="12" t="s">
         <v>133</v>
       </c>
       <c r="E112" s="12" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="F112" s="18">
         <f t="shared" si="10"/>
@@ -9707,13 +9737,13 @@
         <v>110</v>
       </c>
       <c r="B113" s="12" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D113" s="12" t="s">
         <v>133</v>
       </c>
       <c r="E113" s="12" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="F113" s="18">
         <f t="shared" si="10"/>
@@ -9780,7 +9810,7 @@
         <v>133</v>
       </c>
       <c r="E114" s="12" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F114" s="18">
         <f t="shared" si="10"/>
@@ -9844,13 +9874,13 @@
         <v>112</v>
       </c>
       <c r="B115" s="12" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D115" s="12" t="s">
         <v>133</v>
       </c>
       <c r="E115" s="12" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="F115" s="18">
         <f t="shared" si="10"/>
@@ -9913,13 +9943,13 @@
         <v>113</v>
       </c>
       <c r="B116" s="12" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="D116" s="12" t="s">
         <v>133</v>
       </c>
       <c r="E116" s="12" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F116" s="18">
         <f t="shared" si="10"/>
@@ -9973,13 +10003,13 @@
         <v>114</v>
       </c>
       <c r="B117" s="12" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="D117" s="12" t="s">
         <v>133</v>
       </c>
       <c r="E117" s="12" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="F117" s="18">
         <f t="shared" si="10"/>
@@ -10002,13 +10032,13 @@
         <v>115</v>
       </c>
       <c r="B118" s="12" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="D118" s="12" t="s">
         <v>133</v>
       </c>
       <c r="E118" s="12" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="F118" s="18">
         <f t="shared" si="10"/>
@@ -10031,13 +10061,13 @@
         <v>116</v>
       </c>
       <c r="B119" s="12" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D119" s="12" t="s">
         <v>133</v>
       </c>
       <c r="E119" s="12" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F119" s="18">
         <f t="shared" si="10"/>
@@ -10063,7 +10093,7 @@
         <v>133</v>
       </c>
       <c r="E120" s="12" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F120" s="18">
         <f t="shared" si="10"/>
@@ -10081,33 +10111,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:9">
+    <row r="121" spans="1:14">
       <c r="A121" s="12">
         <v>118</v>
       </c>
       <c r="B121" s="12" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D121" s="12" t="s">
         <v>133</v>
       </c>
       <c r="E121" s="12" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F121" s="18">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="G121" s="18">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H121" s="18">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="I121" s="35">
         <v>0</v>
+      </c>
+      <c r="N121" s="12">
+        <f>2*1500</f>
+        <v>3000</v>
       </c>
     </row>
     <row r="122" spans="1:9">
@@ -10115,13 +10149,13 @@
         <v>119</v>
       </c>
       <c r="B122" s="12" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D122" s="12" t="s">
         <v>133</v>
       </c>
       <c r="E122" s="12" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="F122" s="18">
         <f t="shared" si="10"/>
@@ -10147,7 +10181,7 @@
         <v>133</v>
       </c>
       <c r="E123" s="12" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="F123" s="18">
         <f t="shared" si="10"/>
@@ -10170,13 +10204,13 @@
         <v>121</v>
       </c>
       <c r="B124" s="12" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D124" s="12" t="s">
         <v>133</v>
       </c>
       <c r="E124" s="12" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="F124" s="18">
         <f t="shared" si="10"/>
@@ -10199,13 +10233,13 @@
         <v>122</v>
       </c>
       <c r="B125" s="12" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D125" s="12" t="s">
         <v>133</v>
       </c>
       <c r="E125" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F125" s="18">
         <f t="shared" si="10"/>
@@ -10231,7 +10265,7 @@
         <v>133</v>
       </c>
       <c r="E126" s="12" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="F126" s="18">
         <f t="shared" si="10"/>
@@ -10260,7 +10294,7 @@
         <v>133</v>
       </c>
       <c r="E127" s="12" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="F127" s="18">
         <f t="shared" si="10"/>
@@ -10290,7 +10324,7 @@
         <v>133</v>
       </c>
       <c r="E128" s="12" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F128" s="18">
         <f t="shared" si="10"/>
@@ -10313,7 +10347,7 @@
         <v>126</v>
       </c>
       <c r="D129" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F129" s="18">
         <f t="shared" ref="F129:F175" si="13">H129+I129</f>
@@ -10336,13 +10370,13 @@
         <v>127</v>
       </c>
       <c r="B130" s="12" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D130" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E130" s="12" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="F130" s="18">
         <f t="shared" si="13"/>
@@ -10360,30 +10394,34 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:9">
+    <row r="131" spans="1:14">
       <c r="A131" s="12">
         <v>128</v>
       </c>
       <c r="D131" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E131" s="12" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F131" s="18">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="G131" s="18">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H131" s="18">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="I131" s="35">
         <v>0</v>
+      </c>
+      <c r="N131" s="12">
+        <f>1*1500</f>
+        <v>1500</v>
       </c>
     </row>
     <row r="132" spans="1:9">
@@ -10391,7 +10429,7 @@
         <v>129</v>
       </c>
       <c r="D132" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F132" s="18">
         <f t="shared" si="13"/>
@@ -10414,10 +10452,10 @@
         <v>130</v>
       </c>
       <c r="D133" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E133" s="12" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F133" s="18">
         <f t="shared" si="13"/>
@@ -10440,10 +10478,10 @@
         <v>131</v>
       </c>
       <c r="D134" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E134" s="12" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F134" s="18">
         <f t="shared" si="13"/>
@@ -10466,10 +10504,10 @@
         <v>132</v>
       </c>
       <c r="D135" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E135" s="12" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F135" s="18">
         <f t="shared" si="13"/>
@@ -10492,10 +10530,10 @@
         <v>133</v>
       </c>
       <c r="D136" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E136" s="12" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="F136" s="18">
         <f t="shared" si="13"/>
@@ -10518,7 +10556,7 @@
         <v>134</v>
       </c>
       <c r="D137" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F137" s="18">
         <f t="shared" si="13"/>
@@ -10541,10 +10579,10 @@
         <v>135</v>
       </c>
       <c r="D138" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E138" s="12" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="F138" s="18">
         <f t="shared" si="13"/>
@@ -10567,10 +10605,10 @@
         <v>136</v>
       </c>
       <c r="D139" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E139" s="12" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F139" s="18">
         <f t="shared" si="13"/>
@@ -10593,10 +10631,10 @@
         <v>137</v>
       </c>
       <c r="D140" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E140" s="12" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="F140" s="18">
         <f t="shared" si="13"/>
@@ -10619,10 +10657,10 @@
         <v>138</v>
       </c>
       <c r="D141" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E141" s="12" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F141" s="18">
         <f t="shared" si="13"/>
@@ -10645,10 +10683,10 @@
         <v>139</v>
       </c>
       <c r="D142" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E142" s="12" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F142" s="18">
         <f t="shared" si="13"/>
@@ -10671,10 +10709,10 @@
         <v>140</v>
       </c>
       <c r="D143" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E143" s="12" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="F143" s="18">
         <f t="shared" si="13"/>
@@ -10697,10 +10735,10 @@
         <v>141</v>
       </c>
       <c r="D144" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E144" s="12" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="F144" s="18">
         <f t="shared" si="13"/>
@@ -10723,10 +10761,10 @@
         <v>142</v>
       </c>
       <c r="D145" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E145" s="12" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="F145" s="18">
         <f t="shared" si="13"/>
@@ -10749,10 +10787,10 @@
         <v>143</v>
       </c>
       <c r="D146" s="12" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E146" s="12" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="F146" s="18">
         <f t="shared" si="13"/>
@@ -10775,10 +10813,10 @@
         <v>144</v>
       </c>
       <c r="D147" s="12" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E147" s="12" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="F147" s="18">
         <f t="shared" si="13"/>
@@ -10801,10 +10839,10 @@
         <v>145</v>
       </c>
       <c r="D148" s="12" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="E148" s="12" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F148" s="18">
         <f t="shared" si="13"/>
@@ -10827,7 +10865,7 @@
         <v>146</v>
       </c>
       <c r="D149" s="12" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F149" s="18">
         <f t="shared" si="13"/>
@@ -10850,7 +10888,7 @@
         <v>147</v>
       </c>
       <c r="D150" s="12" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F150" s="18">
         <f t="shared" si="13"/>
@@ -10873,10 +10911,10 @@
         <v>148</v>
       </c>
       <c r="D151" s="12" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E151" s="12" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F151" s="18">
         <f t="shared" si="13"/>
@@ -10899,7 +10937,7 @@
         <v>149</v>
       </c>
       <c r="D152" s="12" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F152" s="18">
         <f t="shared" si="13"/>
@@ -10922,10 +10960,10 @@
         <v>150</v>
       </c>
       <c r="D153" s="12" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="E153" s="12" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F153" s="18">
         <f t="shared" si="13"/>
@@ -10952,7 +10990,7 @@
         <v>151</v>
       </c>
       <c r="D154" s="12" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F154" s="18">
         <f t="shared" si="13"/>
@@ -10975,10 +11013,10 @@
         <v>152</v>
       </c>
       <c r="D155" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="E155" s="12" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F155" s="18">
         <f t="shared" si="13"/>
@@ -11001,7 +11039,7 @@
         <v>153</v>
       </c>
       <c r="D156" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F156" s="18">
         <f t="shared" si="13"/>
@@ -11024,7 +11062,7 @@
         <v>154</v>
       </c>
       <c r="D157" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="F157" s="18">
         <f t="shared" si="13"/>
@@ -11090,10 +11128,10 @@
         <v>157</v>
       </c>
       <c r="D160" s="12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="E160" s="12" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F160" s="18">
         <f t="shared" si="13"/>
@@ -11116,10 +11154,10 @@
         <v>158</v>
       </c>
       <c r="D161" s="12" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E161" s="12" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F161" s="18">
         <f t="shared" si="13"/>
@@ -11225,7 +11263,7 @@
         <v>78</v>
       </c>
       <c r="E166" s="12" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F166" s="18">
         <f t="shared" si="13"/>
@@ -11248,10 +11286,10 @@
         <v>164</v>
       </c>
       <c r="D167" s="12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E167" s="12" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F167" s="18">
         <f t="shared" si="13"/>
@@ -11274,10 +11312,10 @@
         <v>165</v>
       </c>
       <c r="D168" s="12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E168" s="12" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F168" s="18">
         <f t="shared" si="13"/>
@@ -11300,10 +11338,10 @@
         <v>166</v>
       </c>
       <c r="D169" s="12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E169" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="F169" s="18">
         <f t="shared" si="13"/>
@@ -11326,10 +11364,10 @@
         <v>167</v>
       </c>
       <c r="D170" s="12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E170" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F170" s="18">
         <f t="shared" si="13"/>
@@ -11352,10 +11390,10 @@
         <v>168</v>
       </c>
       <c r="D171" s="12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E171" s="12" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F171" s="18">
         <f t="shared" si="13"/>
@@ -11378,10 +11416,10 @@
         <v>169</v>
       </c>
       <c r="D172" s="12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E172" s="12" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F172" s="18">
         <f t="shared" si="13"/>
@@ -11404,10 +11442,10 @@
         <v>170</v>
       </c>
       <c r="D173" s="12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E173" s="12" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F173" s="18">
         <f t="shared" si="13"/>
@@ -11430,10 +11468,10 @@
         <v>171</v>
       </c>
       <c r="D174" s="12" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E174" s="12" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F174" s="18">
         <f t="shared" si="13"/>
@@ -11456,10 +11494,10 @@
         <v>172</v>
       </c>
       <c r="D175" s="12" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="E175" s="12" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F175" s="18">
         <f t="shared" si="13"/>
@@ -11492,11 +11530,11 @@
   <dimension ref="A1:BA175"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="6" ySplit="2" topLeftCell="I68" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="6" ySplit="2" topLeftCell="I92" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K73" sqref="K73"/>
+      <selection pane="bottomRight" activeCell="N104" sqref="N104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -11533,7 +11571,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="F1" s="19" t="s">
         <v>3</v>
@@ -11542,7 +11580,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="I1" s="24">
         <v>44378</v>
@@ -11647,14 +11685,14 @@
       <c r="E2" s="20"/>
       <c r="F2" s="21">
         <f>SUM(H3:H1000)</f>
-        <v>27000</v>
+        <v>53000</v>
       </c>
       <c r="G2" s="22" t="s">
         <v>9</v>
       </c>
       <c r="H2" s="21">
         <f>SUM(I2:AM2)</f>
-        <v>27000</v>
+        <v>53000</v>
       </c>
       <c r="I2" s="25">
         <f>SUM(I3:I1000)</f>
@@ -11674,11 +11712,11 @@
       </c>
       <c r="M2" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="N2" s="25">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>11000</v>
       </c>
       <c r="O2" s="25">
         <f t="shared" si="0"/>
@@ -11787,13 +11825,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="C3" s="12">
         <v>1</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="E3" s="12">
         <v>9334066332</v>
@@ -11859,16 +11897,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C4" s="12">
         <v>2</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>10</v>
@@ -11997,13 +12035,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C6" s="12">
         <v>4</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="E6" s="12">
         <v>9102317719</v>
@@ -12073,13 +12111,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C7" s="12">
         <v>5</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="E7" s="12">
         <v>8210924561</v>
@@ -12343,13 +12381,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C11" s="12">
         <v>9</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="E11" s="12">
         <v>9973022718</v>
@@ -12547,13 +12585,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C14" s="12">
         <v>12</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E14" s="12">
         <v>7004740439</v>
@@ -12688,13 +12726,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C16" s="12">
         <v>14</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="E16" s="12">
         <v>7321004323</v>
@@ -12886,13 +12924,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="12" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C19" s="12">
         <v>17</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="E19" s="12">
         <v>9608475282</v>
@@ -12958,13 +12996,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="12" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C20" s="12">
         <v>18</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E20" s="12">
         <v>9661555592</v>
@@ -13030,13 +13068,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="12" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C21" s="12">
         <v>19</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E21" s="12">
         <v>8340523512</v>
@@ -13168,13 +13206,13 @@
         <v>21</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C23" s="12">
         <v>21</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E23" s="12">
         <v>7004478123</v>
@@ -13306,13 +13344,13 @@
         <v>23</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="C25" s="12">
         <v>23</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E25" s="12">
         <v>7006041121</v>
@@ -13325,13 +13363,15 @@
       </c>
       <c r="H25" s="18">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
+      <c r="M25" s="1">
+        <v>1500</v>
+      </c>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
@@ -13378,13 +13418,13 @@
         <v>24</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C26" s="12">
         <v>24</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="E26" s="12">
         <v>8709658240</v>
@@ -13714,13 +13754,13 @@
         <v>29</v>
       </c>
       <c r="B31" s="12" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C31" s="12">
         <v>29</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F31" s="12" t="s">
         <v>37</v>
@@ -13783,13 +13823,13 @@
         <v>30</v>
       </c>
       <c r="B32" s="12" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C32" s="12">
         <v>30</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="F32" s="12" t="s">
         <v>37</v>
@@ -13917,13 +13957,13 @@
         <v>32</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="C34" s="12">
         <v>32</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="F34" s="12" t="s">
         <v>52</v>
@@ -14245,13 +14285,13 @@
         <v>37</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="C39" s="12">
         <v>37</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="F39" s="12" t="s">
         <v>52</v>
@@ -14314,16 +14354,16 @@
         <v>38</v>
       </c>
       <c r="B40" s="12" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="C40" s="12">
         <v>38</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E40" s="12" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="F40" s="12" t="s">
         <v>52</v>
@@ -14704,13 +14744,13 @@
         <v>44</v>
       </c>
       <c r="B46" s="12" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="C46" s="12">
         <v>44</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F46" s="12" t="s">
         <v>65</v>
@@ -14838,13 +14878,13 @@
         <v>46</v>
       </c>
       <c r="B48" s="12" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C48" s="12">
         <v>46</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F48" s="12" t="s">
         <v>65</v>
@@ -14907,13 +14947,13 @@
         <v>47</v>
       </c>
       <c r="B49" s="12" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="C49" s="12">
         <v>47</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="E49" s="12">
         <v>8863097933</v>
@@ -14926,7 +14966,7 @@
       </c>
       <c r="H49" s="18">
         <f t="shared" si="2"/>
-        <v>4500</v>
+        <v>7500</v>
       </c>
       <c r="I49" s="1"/>
       <c r="J49" s="1"/>
@@ -14934,7 +14974,9 @@
         <v>4500</v>
       </c>
       <c r="L49" s="1"/>
-      <c r="M49" s="1"/>
+      <c r="M49" s="1">
+        <v>3000</v>
+      </c>
       <c r="N49" s="1"/>
       <c r="O49" s="1"/>
       <c r="P49" s="1"/>
@@ -14981,13 +15023,13 @@
         <v>48</v>
       </c>
       <c r="B50" s="12" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C50" s="12">
         <v>48</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E50" s="12">
         <v>9835443096</v>
@@ -15053,13 +15095,13 @@
         <v>49</v>
       </c>
       <c r="B51" s="12" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C51" s="12">
         <v>49</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="F51" s="12" t="s">
         <v>65</v>
@@ -15185,13 +15227,13 @@
         <v>51</v>
       </c>
       <c r="B53" s="12" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C53" s="12">
         <v>51</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="F53" s="12" t="s">
         <v>65</v>
@@ -15317,13 +15359,13 @@
         <v>53</v>
       </c>
       <c r="B55" s="12" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="C55" s="12">
         <v>53</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="F55" s="12" t="s">
         <v>65</v>
@@ -15386,13 +15428,13 @@
         <v>54</v>
       </c>
       <c r="B56" s="12" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C56" s="12">
         <v>54</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F56" s="12" t="s">
         <v>65</v>
@@ -15587,13 +15629,13 @@
         <v>57</v>
       </c>
       <c r="B59" s="12" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="C59" s="12">
         <v>57</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="F59" s="12" t="s">
         <v>78</v>
@@ -15782,13 +15824,13 @@
         <v>60</v>
       </c>
       <c r="B62" s="12" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C62" s="12">
         <v>60</v>
       </c>
       <c r="D62" s="12" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E62" s="12">
         <v>9504958065</v>
@@ -15801,14 +15843,16 @@
       </c>
       <c r="H62" s="18">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6000</v>
       </c>
       <c r="I62" s="1"/>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
       <c r="M62" s="1"/>
-      <c r="N62" s="1"/>
+      <c r="N62" s="26">
+        <v>6000</v>
+      </c>
       <c r="O62" s="1"/>
       <c r="P62" s="1"/>
       <c r="Q62" s="1"/>
@@ -15920,16 +15964,16 @@
         <v>62</v>
       </c>
       <c r="B64" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C64" s="12">
         <v>62</v>
       </c>
       <c r="D64" s="12" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="E64" s="12" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="F64" s="12" t="s">
         <v>83</v>
@@ -15992,13 +16036,13 @@
         <v>63</v>
       </c>
       <c r="B65" s="12" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C65" s="12">
         <v>63</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E65" s="12">
         <v>7004399486</v>
@@ -16064,13 +16108,13 @@
         <v>64</v>
       </c>
       <c r="B66" s="12" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="C66" s="12">
         <v>64</v>
       </c>
       <c r="D66" s="12" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F66" s="12" t="s">
         <v>88</v>
@@ -16576,13 +16620,13 @@
         <v>72</v>
       </c>
       <c r="B74" s="12" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="C74" s="12">
         <v>72</v>
       </c>
       <c r="D74" s="12" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E74" s="12">
         <v>8825370430</v>
@@ -16777,13 +16821,13 @@
         <v>75</v>
       </c>
       <c r="B77" s="12" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C77" s="12">
         <v>75</v>
       </c>
       <c r="D77" s="12" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="E77" s="12">
         <v>6200769032</v>
@@ -16849,13 +16893,13 @@
         <v>76</v>
       </c>
       <c r="B78" s="12" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C78" s="12">
         <v>76</v>
       </c>
       <c r="D78" s="12" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="F78" s="12" t="s">
         <v>103</v>
@@ -16918,13 +16962,13 @@
         <v>77</v>
       </c>
       <c r="B79" s="12" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C79" s="12">
         <v>77</v>
       </c>
       <c r="D79" s="12" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="F79" s="12" t="s">
         <v>103</v>
@@ -17047,16 +17091,16 @@
         <v>79</v>
       </c>
       <c r="B81" s="12" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C81" s="12">
         <v>79</v>
       </c>
       <c r="D81" s="12" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="E81" s="12" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="F81" s="12" t="s">
         <v>108</v>
@@ -17302,13 +17346,13 @@
         <v>83</v>
       </c>
       <c r="B85" s="12" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C85" s="12">
         <v>83</v>
       </c>
       <c r="D85" s="12" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="F85" s="12" t="s">
         <v>114</v>
@@ -17439,13 +17483,13 @@
         <v>85</v>
       </c>
       <c r="B87" s="12" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C87" s="12">
         <v>85</v>
       </c>
       <c r="D87" s="12" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E87" s="12">
         <v>7004210181</v>
@@ -17634,13 +17678,13 @@
         <v>88</v>
       </c>
       <c r="B90" s="12" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C90" s="12">
         <v>88</v>
       </c>
       <c r="D90" s="12" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="G90" s="23" t="s">
         <v>121</v>
@@ -18296,16 +18340,21 @@
       <c r="F101" s="12" t="s">
         <v>133</v>
       </c>
+      <c r="G101" s="12" t="s">
+        <v>136</v>
+      </c>
       <c r="H101" s="18">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2000</v>
       </c>
       <c r="I101" s="1"/>
       <c r="J101" s="1"/>
       <c r="K101" s="1"/>
       <c r="L101" s="1"/>
       <c r="M101" s="1"/>
-      <c r="N101" s="1"/>
+      <c r="N101" s="1">
+        <v>2000</v>
+      </c>
       <c r="O101" s="1"/>
       <c r="P101" s="1"/>
       <c r="Q101" s="1"/>
@@ -18352,7 +18401,7 @@
         <v>133</v>
       </c>
       <c r="G102" s="12" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H102" s="18">
         <f t="shared" si="4"/>
@@ -18410,18 +18459,20 @@
         <v>133</v>
       </c>
       <c r="G103" s="12" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H103" s="18">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="I103" s="1"/>
       <c r="J103" s="1"/>
       <c r="K103" s="1"/>
       <c r="L103" s="1"/>
       <c r="M103" s="1"/>
-      <c r="N103" s="1"/>
+      <c r="N103" s="1">
+        <v>3000</v>
+      </c>
       <c r="O103" s="1"/>
       <c r="P103" s="1"/>
       <c r="Q103" s="1"/>
@@ -18468,7 +18519,7 @@
         <v>133</v>
       </c>
       <c r="G104" s="12" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H104" s="18">
         <f t="shared" si="4"/>
@@ -18581,7 +18632,7 @@
         <v>133</v>
       </c>
       <c r="G106" s="12" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H106" s="18">
         <f t="shared" si="4"/>
@@ -18639,17 +18690,19 @@
         <v>133</v>
       </c>
       <c r="G107" s="12" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H107" s="18">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3000</v>
       </c>
       <c r="I107" s="1"/>
       <c r="J107" s="1"/>
       <c r="K107" s="1"/>
       <c r="L107" s="1"/>
-      <c r="M107" s="1"/>
+      <c r="M107" s="1">
+        <v>3000</v>
+      </c>
       <c r="N107" s="1"/>
       <c r="O107" s="1"/>
       <c r="P107" s="1"/>
@@ -18697,7 +18750,7 @@
         <v>133</v>
       </c>
       <c r="G108" s="12" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H108" s="18">
         <f t="shared" si="4"/>
@@ -18755,7 +18808,7 @@
         <v>133</v>
       </c>
       <c r="G109" s="12" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H109" s="18">
         <f t="shared" si="4"/>
@@ -18813,7 +18866,7 @@
         <v>133</v>
       </c>
       <c r="G110" s="12" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H110" s="18">
         <f t="shared" si="4"/>
@@ -18871,7 +18924,7 @@
         <v>133</v>
       </c>
       <c r="G111" s="12" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H111" s="18">
         <f t="shared" si="4"/>
@@ -18929,7 +18982,7 @@
         <v>133</v>
       </c>
       <c r="G112" s="12" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H112" s="18">
         <f t="shared" si="4"/>
@@ -18987,7 +19040,7 @@
         <v>133</v>
       </c>
       <c r="G113" s="12" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H113" s="18">
         <f t="shared" si="4"/>
@@ -19002,7 +19055,7 @@
         <v>133</v>
       </c>
       <c r="G114" s="12" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H114" s="18">
         <f t="shared" si="4"/>
@@ -19017,7 +19070,7 @@
         <v>133</v>
       </c>
       <c r="G115" s="12" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H115" s="18">
         <f t="shared" si="4"/>
@@ -19032,7 +19085,7 @@
         <v>133</v>
       </c>
       <c r="G116" s="12" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H116" s="18">
         <f t="shared" si="4"/>
@@ -19047,7 +19100,7 @@
         <v>133</v>
       </c>
       <c r="G117" s="12" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H117" s="18">
         <f t="shared" si="4"/>
@@ -19062,7 +19115,7 @@
         <v>133</v>
       </c>
       <c r="G118" s="12" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H118" s="18">
         <f t="shared" si="4"/>
@@ -19077,7 +19130,7 @@
         <v>133</v>
       </c>
       <c r="G119" s="12" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H119" s="18">
         <f t="shared" si="4"/>
@@ -19092,14 +19145,14 @@
         <v>133</v>
       </c>
       <c r="G120" s="12" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H120" s="18">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="3:8">
+    <row r="121" spans="3:13">
       <c r="C121" s="12">
         <v>118</v>
       </c>
@@ -19107,11 +19160,14 @@
         <v>133</v>
       </c>
       <c r="G121" s="12" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H121" s="18">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3000</v>
+      </c>
+      <c r="M121" s="12">
+        <v>3000</v>
       </c>
     </row>
     <row r="122" spans="3:8">
@@ -19122,7 +19178,7 @@
         <v>133</v>
       </c>
       <c r="G122" s="12" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H122" s="18">
         <f t="shared" si="4"/>
@@ -19137,7 +19193,7 @@
         <v>133</v>
       </c>
       <c r="G123" s="12" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H123" s="18">
         <f t="shared" si="4"/>
@@ -19152,7 +19208,7 @@
         <v>133</v>
       </c>
       <c r="G124" s="12" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H124" s="18">
         <f t="shared" si="4"/>
@@ -19167,7 +19223,7 @@
         <v>133</v>
       </c>
       <c r="G125" s="12" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H125" s="18">
         <f t="shared" si="4"/>
@@ -19182,14 +19238,14 @@
         <v>133</v>
       </c>
       <c r="G126" s="12" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H126" s="18">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="3:8">
+    <row r="127" spans="3:13">
       <c r="C127" s="12">
         <v>124</v>
       </c>
@@ -19197,11 +19253,14 @@
         <v>133</v>
       </c>
       <c r="G127" s="12" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H127" s="18">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>3000</v>
+      </c>
+      <c r="M127" s="12">
+        <v>3000</v>
       </c>
     </row>
     <row r="128" spans="3:8">
@@ -19212,7 +19271,7 @@
         <v>133</v>
       </c>
       <c r="G128" s="12" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H128" s="18">
         <f t="shared" si="4"/>
@@ -19224,7 +19283,7 @@
         <v>126</v>
       </c>
       <c r="F129" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H129" s="18">
         <f t="shared" ref="H129:H175" si="5">SUM(I129:AM129)</f>
@@ -19236,29 +19295,32 @@
         <v>127</v>
       </c>
       <c r="F130" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G130" s="12" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H130" s="18">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="3:8">
+    <row r="131" spans="3:13">
       <c r="C131" s="12">
         <v>128</v>
       </c>
       <c r="F131" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G131" s="12" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H131" s="18">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1500</v>
+      </c>
+      <c r="M131" s="12">
+        <v>1500</v>
       </c>
     </row>
     <row r="132" spans="3:8">
@@ -19266,7 +19328,7 @@
         <v>129</v>
       </c>
       <c r="F132" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H132" s="18">
         <f t="shared" si="5"/>
@@ -19278,10 +19340,10 @@
         <v>130</v>
       </c>
       <c r="F133" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G133" s="12" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H133" s="18">
         <f t="shared" si="5"/>
@@ -19293,10 +19355,10 @@
         <v>131</v>
       </c>
       <c r="F134" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G134" s="12" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H134" s="18">
         <f t="shared" si="5"/>
@@ -19308,10 +19370,10 @@
         <v>132</v>
       </c>
       <c r="F135" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G135" s="12" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H135" s="18">
         <f t="shared" si="5"/>
@@ -19323,10 +19385,10 @@
         <v>133</v>
       </c>
       <c r="F136" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G136" s="12" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H136" s="18">
         <f t="shared" si="5"/>
@@ -19338,7 +19400,7 @@
         <v>134</v>
       </c>
       <c r="F137" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H137" s="18">
         <f t="shared" si="5"/>
@@ -19350,10 +19412,10 @@
         <v>135</v>
       </c>
       <c r="F138" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G138" s="12" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H138" s="18">
         <f t="shared" si="5"/>
@@ -19365,10 +19427,10 @@
         <v>136</v>
       </c>
       <c r="F139" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G139" s="12" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H139" s="18">
         <f t="shared" si="5"/>
@@ -19380,10 +19442,10 @@
         <v>137</v>
       </c>
       <c r="F140" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G140" s="12" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H140" s="18">
         <f t="shared" si="5"/>
@@ -19395,10 +19457,10 @@
         <v>138</v>
       </c>
       <c r="F141" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G141" s="12" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="H141" s="18">
         <f t="shared" si="5"/>
@@ -19410,10 +19472,10 @@
         <v>139</v>
       </c>
       <c r="F142" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G142" s="12" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H142" s="18">
         <f t="shared" si="5"/>
@@ -19425,10 +19487,10 @@
         <v>140</v>
       </c>
       <c r="F143" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G143" s="12" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H143" s="18">
         <f t="shared" si="5"/>
@@ -19440,10 +19502,10 @@
         <v>141</v>
       </c>
       <c r="F144" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G144" s="12" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H144" s="18">
         <f t="shared" si="5"/>
@@ -19455,10 +19517,10 @@
         <v>142</v>
       </c>
       <c r="F145" s="12" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G145" s="12" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="H145" s="18">
         <f t="shared" si="5"/>
@@ -19470,10 +19532,10 @@
         <v>143</v>
       </c>
       <c r="F146" s="12" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="G146" s="12" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H146" s="18">
         <f t="shared" si="5"/>
@@ -19485,10 +19547,10 @@
         <v>144</v>
       </c>
       <c r="F147" s="12" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="G147" s="12" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H147" s="18">
         <f t="shared" si="5"/>
@@ -19500,10 +19562,10 @@
         <v>145</v>
       </c>
       <c r="F148" s="12" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="G148" s="12" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="H148" s="18">
         <f t="shared" si="5"/>
@@ -19515,7 +19577,7 @@
         <v>146</v>
       </c>
       <c r="F149" s="12" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H149" s="18">
         <f t="shared" si="5"/>
@@ -19527,7 +19589,7 @@
         <v>147</v>
       </c>
       <c r="F150" s="12" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H150" s="18">
         <f t="shared" si="5"/>
@@ -19539,10 +19601,10 @@
         <v>148</v>
       </c>
       <c r="F151" s="12" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G151" s="12" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="H151" s="18">
         <f t="shared" si="5"/>
@@ -19554,7 +19616,7 @@
         <v>149</v>
       </c>
       <c r="F152" s="12" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H152" s="18">
         <f t="shared" si="5"/>
@@ -19566,10 +19628,10 @@
         <v>150</v>
       </c>
       <c r="F153" s="12" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G153" s="12" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="H153" s="18">
         <f t="shared" si="5"/>
@@ -19581,7 +19643,7 @@
         <v>151</v>
       </c>
       <c r="F154" s="12" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H154" s="18">
         <f t="shared" si="5"/>
@@ -19593,10 +19655,10 @@
         <v>152</v>
       </c>
       <c r="F155" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G155" s="12" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="H155" s="18">
         <f t="shared" si="5"/>
@@ -19608,7 +19670,7 @@
         <v>153</v>
       </c>
       <c r="F156" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H156" s="18">
         <f t="shared" si="5"/>
@@ -19620,7 +19682,7 @@
         <v>154</v>
       </c>
       <c r="F157" s="12" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H157" s="18">
         <f t="shared" si="5"/>
@@ -19653,10 +19715,10 @@
         <v>157</v>
       </c>
       <c r="F160" s="12" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G160" s="12" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H160" s="18">
         <f t="shared" si="5"/>
@@ -19668,10 +19730,10 @@
         <v>158</v>
       </c>
       <c r="F161" s="12" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="G161" s="12" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H161" s="18">
         <f t="shared" si="5"/>
@@ -19722,7 +19784,7 @@
         <v>78</v>
       </c>
       <c r="G166" s="12" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="H166" s="18">
         <f t="shared" si="5"/>
@@ -19734,10 +19796,10 @@
         <v>164</v>
       </c>
       <c r="F167" s="12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G167" s="12" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="H167" s="18">
         <f t="shared" si="5"/>
@@ -19749,10 +19811,10 @@
         <v>165</v>
       </c>
       <c r="F168" s="12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G168" s="12" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="H168" s="18">
         <f t="shared" si="5"/>
@@ -19764,10 +19826,10 @@
         <v>166</v>
       </c>
       <c r="F169" s="12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G169" s="12" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="H169" s="18">
         <f t="shared" si="5"/>
@@ -19779,10 +19841,10 @@
         <v>167</v>
       </c>
       <c r="F170" s="12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G170" s="12" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H170" s="18">
         <f t="shared" si="5"/>
@@ -19794,10 +19856,10 @@
         <v>168</v>
       </c>
       <c r="F171" s="12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G171" s="12" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="H171" s="18">
         <f t="shared" si="5"/>
@@ -19809,10 +19871,10 @@
         <v>169</v>
       </c>
       <c r="F172" s="12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G172" s="12" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="H172" s="18">
         <f t="shared" si="5"/>
@@ -19824,10 +19886,10 @@
         <v>170</v>
       </c>
       <c r="F173" s="12" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="G173" s="12" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H173" s="18">
         <f t="shared" si="5"/>
@@ -19839,10 +19901,10 @@
         <v>171</v>
       </c>
       <c r="F174" s="12" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G174" s="12" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H174" s="18">
         <f t="shared" si="5"/>
@@ -19854,10 +19916,10 @@
         <v>172</v>
       </c>
       <c r="F175" s="12" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G175" s="12" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H175" s="18">
         <f t="shared" si="5"/>
@@ -19879,7 +19941,7 @@
   <dimension ref="A1:E175"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="E98" sqref="E98"/>
     </sheetView>
@@ -19900,32 +19962,32 @@
         <v>3</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E1" s="4">
         <f>ROUND(SUM(D3:D1000),0)</f>
-        <v>83500</v>
+        <v>78500</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6" t="s">
-        <v>9</v>
+        <v>265</v>
       </c>
       <c r="D2" s="7">
         <f>Orders!F2-Collection!H2</f>
-        <v>83500</v>
+        <v>78500</v>
       </c>
       <c r="E2" s="8">
         <f>SUM(D3:D97)</f>
-        <v>79000</v>
+        <v>76000</v>
       </c>
     </row>
     <row r="3" hidden="1" spans="1:4">
@@ -20558,7 +20620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" hidden="1" spans="1:4">
+    <row r="45" spans="1:4">
       <c r="A45" s="9" t="s">
         <v>52</v>
       </c>
@@ -20570,7 +20632,7 @@
       </c>
       <c r="D45" s="11">
         <f>Orders!F45-Collection!H45</f>
-        <v>0</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="46" hidden="1" spans="1:4">
@@ -20813,7 +20875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" hidden="1" spans="1:4">
       <c r="A62" s="9" t="s">
         <v>83</v>
       </c>
@@ -20825,7 +20887,7 @@
       </c>
       <c r="D62" s="11">
         <f>Orders!F62-Collection!H62</f>
-        <v>6000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" hidden="1" spans="1:4">
@@ -21249,7 +21311,7 @@
     </row>
     <row r="92" hidden="1" spans="1:4">
       <c r="A92" s="9" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B92" s="9">
         <v>7992363545</v>
@@ -21323,7 +21385,7 @@
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="15" t="s">
-        <v>131</v>
+        <v>267</v>
       </c>
       <c r="B98" s="15"/>
       <c r="C98" s="15"/>
@@ -21332,7 +21394,7 @@
       </c>
       <c r="E98" s="8">
         <f>SUM(D99:D175)</f>
-        <v>4500</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="99" hidden="1" spans="1:4">
@@ -21363,15 +21425,17 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" hidden="1" spans="1:4">
+    <row r="101" spans="1:4">
       <c r="A101" s="9" t="s">
         <v>133</v>
       </c>
       <c r="B101" s="14"/>
-      <c r="C101" s="9"/>
+      <c r="C101" s="12" t="s">
+        <v>136</v>
+      </c>
       <c r="D101" s="11">
         <f>Orders!F101-Collection!H101</f>
-        <v>0</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="102" hidden="1" spans="1:4">
@@ -21380,7 +21444,7 @@
       </c>
       <c r="B102" s="14"/>
       <c r="C102" s="9" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="D102" s="11">
         <f>Orders!F102-Collection!H102</f>
@@ -21395,7 +21459,7 @@
         <v>9122190230</v>
       </c>
       <c r="C103" s="9" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="D103" s="11">
         <f>Orders!F103-Collection!H103</f>
@@ -21410,7 +21474,7 @@
         <v>9122242352</v>
       </c>
       <c r="C104" s="9" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="D104" s="11">
         <f>Orders!F104-Collection!H104</f>
@@ -21434,7 +21498,7 @@
       </c>
       <c r="B106" s="14"/>
       <c r="C106" s="9" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D106" s="11">
         <f>Orders!F106-Collection!H106</f>
@@ -21449,7 +21513,7 @@
         <v>7979719608</v>
       </c>
       <c r="C107" s="9" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="D107" s="11">
         <f>Orders!F107-Collection!H107</f>
@@ -21462,7 +21526,7 @@
       </c>
       <c r="B108" s="14"/>
       <c r="C108" s="9" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D108" s="11">
         <f>Orders!F108-Collection!H108</f>
@@ -21475,7 +21539,7 @@
       </c>
       <c r="B109" s="14"/>
       <c r="C109" s="9" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="D109" s="11">
         <f>Orders!F109-Collection!H109</f>
@@ -21488,7 +21552,7 @@
       </c>
       <c r="B110" s="14"/>
       <c r="C110" s="9" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="D110" s="11">
         <f>Orders!F110-Collection!H110</f>
@@ -21503,7 +21567,7 @@
         <v>9006359166</v>
       </c>
       <c r="C111" s="9" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D111" s="11">
         <f>Orders!F111-Collection!H111</f>
@@ -21518,7 +21582,7 @@
         <v>8210148576</v>
       </c>
       <c r="C112" s="9" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D112" s="11">
         <f>Orders!F112-Collection!H112</f>
@@ -21533,7 +21597,7 @@
         <v>7258828840</v>
       </c>
       <c r="C113" s="9" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D113" s="11">
         <f>Orders!F113-Collection!H113</f>
@@ -21546,7 +21610,7 @@
       </c>
       <c r="B114" s="14"/>
       <c r="C114" s="9" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D114" s="11">
         <f>Orders!F114-Collection!H114</f>
@@ -21561,7 +21625,7 @@
         <v>9852620786</v>
       </c>
       <c r="C115" s="9" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D115" s="11">
         <f>Orders!F115-Collection!H115</f>
@@ -21576,7 +21640,7 @@
         <v>7004129753</v>
       </c>
       <c r="C116" s="9" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D116" s="11">
         <f>Orders!F116-Collection!H116</f>
@@ -21591,7 +21655,7 @@
         <v>7004308089</v>
       </c>
       <c r="C117" s="9" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D117" s="11">
         <f>Orders!F117-Collection!H117</f>
@@ -21606,7 +21670,7 @@
         <v>748803334</v>
       </c>
       <c r="C118" s="9" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="D118" s="11">
         <f>Orders!F118-Collection!H118</f>
@@ -21621,7 +21685,7 @@
         <v>9199240992</v>
       </c>
       <c r="C119" s="9" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D119" s="11">
         <f>Orders!F119-Collection!H119</f>
@@ -21634,7 +21698,7 @@
       </c>
       <c r="B120" s="14"/>
       <c r="C120" s="9" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="D120" s="11">
         <f>Orders!F120-Collection!H120</f>
@@ -21649,7 +21713,7 @@
         <v>9931256580</v>
       </c>
       <c r="C121" s="9" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="D121" s="11">
         <f>Orders!F121-Collection!H121</f>
@@ -21664,7 +21728,7 @@
         <v>9931070730</v>
       </c>
       <c r="C122" s="9" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D122" s="11">
         <f>Orders!F122-Collection!H122</f>
@@ -21677,7 +21741,7 @@
       </c>
       <c r="B123" s="14"/>
       <c r="C123" s="9" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D123" s="11">
         <f>Orders!F123-Collection!H123</f>
@@ -21692,7 +21756,7 @@
         <v>9852792631</v>
       </c>
       <c r="C124" s="9" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="D124" s="11">
         <f>Orders!F124-Collection!H124</f>
@@ -21707,7 +21771,7 @@
         <v>7004129804</v>
       </c>
       <c r="C125" s="9" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D125" s="11">
         <f>Orders!F125-Collection!H125</f>
@@ -21720,14 +21784,14 @@
       </c>
       <c r="B126" s="14"/>
       <c r="C126" s="9" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D126" s="11">
         <f>Orders!F126-Collection!H126</f>
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:4">
+    <row r="127" hidden="1" spans="1:4">
       <c r="A127" s="9" t="s">
         <v>133</v>
       </c>
@@ -21735,11 +21799,11 @@
         <v>8235940652</v>
       </c>
       <c r="C127" s="9" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D127" s="11">
         <f>Orders!F127-Collection!H127</f>
-        <v>3000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128" hidden="1" spans="1:4">
@@ -21748,7 +21812,7 @@
       </c>
       <c r="B128" s="14"/>
       <c r="C128" s="9" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D128" s="11">
         <f>Orders!F128-Collection!H128</f>
@@ -21757,7 +21821,7 @@
     </row>
     <row r="129" hidden="1" spans="1:4">
       <c r="A129" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B129" s="14"/>
       <c r="C129" s="9"/>
@@ -21768,13 +21832,13 @@
     </row>
     <row r="130" hidden="1" spans="1:4">
       <c r="A130" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B130" s="14">
         <v>9097671230</v>
       </c>
       <c r="C130" s="9" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="D130" s="11">
         <f>Orders!F130-Collection!H130</f>
@@ -21783,13 +21847,13 @@
     </row>
     <row r="131" hidden="1" spans="1:4">
       <c r="A131" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B131" s="14">
         <v>7482908246</v>
       </c>
       <c r="C131" s="9" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D131" s="11">
         <f>Orders!F131-Collection!H131</f>
@@ -21798,7 +21862,7 @@
     </row>
     <row r="132" hidden="1" spans="1:4">
       <c r="A132" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B132" s="14"/>
       <c r="C132" s="9"/>
@@ -21809,13 +21873,13 @@
     </row>
     <row r="133" hidden="1" spans="1:4">
       <c r="A133" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B133" s="14">
         <v>9939518710</v>
       </c>
       <c r="C133" s="9" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="D133" s="11">
         <f>Orders!F133-Collection!H133</f>
@@ -21824,13 +21888,13 @@
     </row>
     <row r="134" hidden="1" spans="1:4">
       <c r="A134" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B134" s="14">
         <v>8340109140</v>
       </c>
       <c r="C134" s="9" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D134" s="11">
         <f>Orders!F134-Collection!H134</f>
@@ -21839,13 +21903,13 @@
     </row>
     <row r="135" hidden="1" spans="1:4">
       <c r="A135" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B135" s="14">
         <v>7004763796</v>
       </c>
       <c r="C135" s="9" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D135" s="11">
         <f>Orders!F135-Collection!H135</f>
@@ -21854,11 +21918,11 @@
     </row>
     <row r="136" hidden="1" spans="1:4">
       <c r="A136" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B136" s="14"/>
       <c r="C136" s="9" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D136" s="11">
         <f>Orders!F136-Collection!H136</f>
@@ -21867,7 +21931,7 @@
     </row>
     <row r="137" hidden="1" spans="1:4">
       <c r="A137" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B137" s="14">
         <v>7033228726</v>
@@ -21880,11 +21944,11 @@
     </row>
     <row r="138" hidden="1" spans="1:4">
       <c r="A138" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B138" s="14"/>
       <c r="C138" s="9" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D138" s="11">
         <f>Orders!F138-Collection!H138</f>
@@ -21893,11 +21957,11 @@
     </row>
     <row r="139" hidden="1" spans="1:4">
       <c r="A139" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B139" s="14"/>
       <c r="C139" s="9" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="D139" s="11">
         <f>Orders!F139-Collection!H139</f>
@@ -21906,13 +21970,13 @@
     </row>
     <row r="140" hidden="1" spans="1:4">
       <c r="A140" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B140" s="14">
         <v>8825232517</v>
       </c>
       <c r="C140" s="9" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D140" s="11">
         <f>Orders!F140-Collection!H140</f>
@@ -21921,13 +21985,13 @@
     </row>
     <row r="141" hidden="1" spans="1:4">
       <c r="A141" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B141" s="14">
         <v>9939163568</v>
       </c>
       <c r="C141" s="9" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="D141" s="11">
         <f>Orders!F141-Collection!H141</f>
@@ -21936,13 +22000,13 @@
     </row>
     <row r="142" hidden="1" spans="1:4">
       <c r="A142" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B142" s="14">
         <v>8804656537</v>
       </c>
       <c r="C142" s="9" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="D142" s="11">
         <f>Orders!F142-Collection!H142</f>
@@ -21951,13 +22015,13 @@
     </row>
     <row r="143" hidden="1" spans="1:4">
       <c r="A143" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B143" s="14">
         <v>9798383030</v>
       </c>
       <c r="C143" s="9" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="D143" s="11">
         <f>Orders!F143-Collection!H143</f>
@@ -21966,13 +22030,13 @@
     </row>
     <row r="144" hidden="1" spans="1:4">
       <c r="A144" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B144" s="14">
         <v>9801442328</v>
       </c>
       <c r="C144" s="9" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="D144" s="11">
         <f>Orders!F144-Collection!H144</f>
@@ -21981,11 +22045,11 @@
     </row>
     <row r="145" hidden="1" spans="1:4">
       <c r="A145" s="9" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B145" s="14"/>
       <c r="C145" s="9" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="D145" s="11">
         <f>Orders!F145-Collection!H145</f>
@@ -21994,13 +22058,13 @@
     </row>
     <row r="146" hidden="1" spans="1:4">
       <c r="A146" s="9" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B146" s="14">
         <v>6207066085</v>
       </c>
       <c r="C146" s="9" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="D146" s="11">
         <f>Orders!F146-Collection!H146</f>
@@ -22009,11 +22073,11 @@
     </row>
     <row r="147" hidden="1" spans="1:4">
       <c r="A147" s="9" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B147" s="14"/>
       <c r="C147" s="9" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="D147" s="11">
         <f>Orders!F147-Collection!H147</f>
@@ -22022,13 +22086,13 @@
     </row>
     <row r="148" hidden="1" spans="1:4">
       <c r="A148" s="9" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B148" s="14">
         <v>8207701228</v>
       </c>
       <c r="C148" s="9" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="D148" s="11">
         <f>Orders!F148-Collection!H148</f>
@@ -22037,7 +22101,7 @@
     </row>
     <row r="149" hidden="1" spans="1:4">
       <c r="A149" s="9" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B149" s="14"/>
       <c r="C149" s="9"/>
@@ -22048,7 +22112,7 @@
     </row>
     <row r="150" hidden="1" spans="1:4">
       <c r="A150" s="9" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B150" s="14"/>
       <c r="C150" s="9"/>
@@ -22059,13 +22123,13 @@
     </row>
     <row r="151" hidden="1" spans="1:4">
       <c r="A151" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B151" s="14">
         <v>9507432307</v>
       </c>
       <c r="C151" s="9" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D151" s="11">
         <f>Orders!F151-Collection!H151</f>
@@ -22074,7 +22138,7 @@
     </row>
     <row r="152" hidden="1" spans="1:4">
       <c r="A152" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B152" s="14"/>
       <c r="C152" s="9"/>
@@ -22085,13 +22149,13 @@
     </row>
     <row r="153" spans="1:4">
       <c r="A153" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B153" s="14">
         <v>9113391144</v>
       </c>
       <c r="C153" s="9" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D153" s="11">
         <f>Orders!F153-Collection!H153</f>
@@ -22100,7 +22164,7 @@
     </row>
     <row r="154" hidden="1" spans="1:4">
       <c r="A154" s="9" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B154" s="14"/>
       <c r="C154" s="9"/>
@@ -22111,11 +22175,11 @@
     </row>
     <row r="155" hidden="1" spans="1:4">
       <c r="A155" s="9" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B155" s="14"/>
       <c r="C155" s="9" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D155" s="11">
         <f>Orders!F155-Collection!H155</f>
@@ -22124,7 +22188,7 @@
     </row>
     <row r="156" hidden="1" spans="1:4">
       <c r="A156" s="9" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B156" s="14"/>
       <c r="C156" s="9"/>
@@ -22135,7 +22199,7 @@
     </row>
     <row r="157" hidden="1" spans="1:4">
       <c r="A157" s="9" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B157" s="14"/>
       <c r="C157" s="9"/>
@@ -22166,13 +22230,13 @@
     </row>
     <row r="160" hidden="1" spans="1:4">
       <c r="A160" s="9" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B160" s="14">
         <v>9110027071</v>
       </c>
       <c r="C160" s="9" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="D160" s="11">
         <f>Orders!F160-Collection!H160</f>
@@ -22181,13 +22245,13 @@
     </row>
     <row r="161" hidden="1" spans="1:4">
       <c r="A161" s="9" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B161" s="14">
         <v>8210849560</v>
       </c>
       <c r="C161" s="9" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D161" s="11">
         <f>Orders!F161-Collection!H161</f>
@@ -22236,7 +22300,7 @@
       </c>
       <c r="B166" s="14"/>
       <c r="C166" s="9" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="D166" s="11">
         <f>Orders!F166-Collection!H166</f>
@@ -22245,13 +22309,13 @@
     </row>
     <row r="167" hidden="1" spans="1:4">
       <c r="A167" s="9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B167" s="14">
         <v>7903210589</v>
       </c>
       <c r="C167" s="9" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D167" s="11">
         <f>Orders!F167-Collection!H167</f>
@@ -22260,13 +22324,13 @@
     </row>
     <row r="168" hidden="1" spans="1:4">
       <c r="A168" s="9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B168" s="14">
         <v>6203201991</v>
       </c>
       <c r="C168" s="9" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D168" s="11">
         <f>Orders!F168-Collection!H168</f>
@@ -22275,13 +22339,13 @@
     </row>
     <row r="169" hidden="1" spans="1:4">
       <c r="A169" s="9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B169" s="14">
         <v>7903748069</v>
       </c>
       <c r="C169" s="9" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D169" s="11">
         <f>Orders!F169-Collection!H169</f>
@@ -22290,13 +22354,13 @@
     </row>
     <row r="170" hidden="1" spans="1:4">
       <c r="A170" s="9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B170" s="14">
         <v>8709003781</v>
       </c>
       <c r="C170" s="9" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D170" s="11">
         <f>Orders!F170-Collection!H170</f>
@@ -22305,13 +22369,13 @@
     </row>
     <row r="171" hidden="1" spans="1:4">
       <c r="A171" s="9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B171" s="14">
         <v>8789050082</v>
       </c>
       <c r="C171" s="9" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="D171" s="11">
         <f>Orders!F171-Collection!H171</f>
@@ -22320,13 +22384,13 @@
     </row>
     <row r="172" hidden="1" spans="1:4">
       <c r="A172" s="9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B172" s="14">
         <v>8002924498</v>
       </c>
       <c r="C172" s="9" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D172" s="11">
         <f>Orders!F172-Collection!H172</f>
@@ -22335,13 +22399,13 @@
     </row>
     <row r="173" hidden="1" spans="1:4">
       <c r="A173" s="9" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B173" s="14">
         <v>7050470759</v>
       </c>
       <c r="C173" s="9" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D173" s="11">
         <f>Orders!F173-Collection!H173</f>
@@ -22350,11 +22414,11 @@
     </row>
     <row r="174" hidden="1" spans="1:4">
       <c r="A174" s="9" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B174" s="14"/>
       <c r="C174" s="9" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D174" s="11">
         <f>Orders!F174-Collection!H174</f>
@@ -22363,13 +22427,13 @@
     </row>
     <row r="175" hidden="1" spans="1:4">
       <c r="A175" s="9" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B175" s="14">
         <v>9852299198</v>
       </c>
       <c r="C175" s="9" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D175" s="11">
         <f>Orders!F175-Collection!H175</f>
@@ -22380,6 +22444,7 @@
   <autoFilter ref="A1:D175">
     <filterColumn colId="3">
       <filters>
+        <filter val="1000"/>
         <filter val="1500"/>
         <filter val="2000"/>
         <filter val="2500"/>
@@ -22389,7 +22454,7 @@
         <filter val="6000"/>
         <filter val="11000"/>
         <filter val="15000"/>
-        <filter val="83500"/>
+        <filter val="78500"/>
         <filter val="0.1"/>
       </filters>
     </filterColumn>

</xml_diff>